<commit_message>
🟡 Main.py - Organizando código
</commit_message>
<xml_diff>
--- a/Excel/AutoTransfer.xlsx
+++ b/Excel/AutoTransfer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodri\Desktop\AutoTransfer\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8010F3A-8A2A-4655-BBB8-1BB7AB656459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AEC1743-1E81-4ED1-8554-CD9D6DEA5FA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CD87EC71-DDA9-4746-BD85-56A81A6FFDD5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Origem</t>
   </si>
@@ -44,90 +44,15 @@
     <t>Destino</t>
   </si>
   <si>
-    <t>C:\Users\rodri\Desktop\DestinoAutoTransfer\CPC-24</t>
-  </si>
-  <si>
-    <t>C:\Users\rodri\Desktop\DestinoAutoTransfer\CPC-27</t>
-  </si>
-  <si>
-    <t>C:\Users\rodri\Desktop\DestinoAutoTransfer\CPC-29</t>
-  </si>
-  <si>
-    <t>C:\Users\rodri\Desktop\DestinoAutoTransfer\CPC-30</t>
-  </si>
-  <si>
-    <t>C:\Users\rodri\Desktop\DestinoAutoTransfer\CPC-31</t>
-  </si>
-  <si>
-    <t>C:\Users\rodri\Desktop\DestinoAutoTransfer\CPC-32</t>
-  </si>
-  <si>
-    <t>C:\Users\rodri\Desktop\DestinoAutoTransfer\CPC-33</t>
-  </si>
-  <si>
-    <t>C:\Users\rodri\Desktop\DestinoAutoTransfer\CPC-35</t>
-  </si>
-  <si>
-    <t>C:\Users\rodri\Desktop\DestinoAutoTransfer\CPC-36</t>
-  </si>
-  <si>
-    <t>C:\Users\rodri\Desktop\DestinoAutoTransfer\CPC-37</t>
-  </si>
-  <si>
-    <t>C:\Users\rodri\Desktop\DestinoAutoTransfer\CPC-38</t>
-  </si>
-  <si>
-    <t>C:\Users\rodri\Desktop\DestinoAutoTransfer\CPC-39</t>
-  </si>
-  <si>
-    <t>C:\Users\rodri\Desktop\DestinoAutoTransfer\CPC-40</t>
-  </si>
-  <si>
-    <t>C:\Users\rodri\Desktop\DestinoAutoTransfer\CPC-41</t>
-  </si>
-  <si>
-    <t>C:\Users\rodri\Desktop\DestinoAutoTransfer\CPC-42</t>
-  </si>
-  <si>
-    <t>C:\Users\rodri\Desktop\DestinoAutoTransfer\CPC-43</t>
-  </si>
-  <si>
-    <t>C:\Users\rodri\Desktop\DestinoAutoTransfer\CPC-44</t>
-  </si>
-  <si>
-    <t>C:\Users\rodri\Desktop\DestinoAutoTransfer\CPC-45</t>
-  </si>
-  <si>
-    <t>C:\Users\rodri\Desktop\DestinoAutoTransfer\CPC-46</t>
-  </si>
-  <si>
-    <t>C:\Users\rodri\Desktop\DestinoAutoTransfer\CPC-47</t>
-  </si>
-  <si>
-    <t>C:\Users\rodri\Desktop\DestinoAutoTransfer\CPC-48</t>
-  </si>
-  <si>
-    <t>C:\Users\rodri\Desktop\DestinoAutoTransfer\CPC-49</t>
-  </si>
-  <si>
-    <t>C:\Users\rodri\Desktop\DestinoAutoTransfer\CPC-50</t>
-  </si>
-  <si>
     <t>C:\Users\rodri\Desktop\TesteAutoTransfer\IHA-50\ArquivoTransfer 2.txt</t>
   </si>
   <si>
     <t>C:\Users\rodri\Desktop\TesteAutoTransfer\IHA-9\ArquivoTransfer 1.txt</t>
   </si>
   <si>
-    <t>C:\Users\rodri\Desktop\DestinoAutoTransfer\CPC-22\ola</t>
-  </si>
-  <si>
     <t>C:\Users\rodri\Desktop\DestinoAutoTransfer\CPC-20/Felipe/Gonçalves</t>
   </si>
   <si>
-    <t>C:\Users\rodri\Desktop\DestinoAutoTransfer\CPC-21/Anana/banana/gelada/Comida</t>
-  </si>
-  <si>
     <t>C:\Users\rodri\Desktop\DestinoAutoTransfer\CPC-23/GUILHRTMR/GDG</t>
   </si>
   <si>
@@ -149,23 +74,29 @@
     <t>CPC-500</t>
   </si>
   <si>
-    <t>C:\Users\rodri\Desktop\DestinoAutoTransfer\CPC-24\BANANA</t>
-  </si>
-  <si>
-    <t>C:\Users\rodri\Desktop\DestinoAutoTransfer\CPC-28\\\\\</t>
-  </si>
-  <si>
-    <t>C:\Users\rodri\Desktop\DestinoAutoTransfer\CPC-33/1</t>
-  </si>
-  <si>
     <t>C:\Users\rodri\Desktop\TesteAutoTransfer\IHA-50</t>
+  </si>
+  <si>
+    <t>C:\Users\rodri\Desktop\DestinoAutoTransfer\CPC-21</t>
+  </si>
+  <si>
+    <t>C:\Users\rodri\Desktop\TesteAutoTransfer\IHA-51</t>
+  </si>
+  <si>
+    <t>C:\Users\rodri\Desktop\TesteAutoTransfer\IHA-52</t>
+  </si>
+  <si>
+    <t>dsadasda</t>
+  </si>
+  <si>
+    <t>C:\Users\rodri\Desktop\DestinoAutoTransfer\CPC-23/GUILHRTMR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -185,6 +116,12 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -239,9 +176,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -576,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63FED6A7-0BE3-45AB-AE4B-3006960D31A5}">
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -598,272 +533,75 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="1" t="str">
-        <f>CONCATENATE(D7,"\",E7,"\",F7,"\",G7,"\",H7,"\",I7)</f>
-        <v>C:\Users\rodri\Desktop\DestinoAutoTransfer\CPC-500</v>
+        <v>2</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="F7" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="G7" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="H7" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="I7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>24</v>
-      </c>
+    <row r="30" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D30" s="3"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>